<commit_message>
Changed the excel spreadsheet's users/roles to match what's in the database.
</commit_message>
<xml_diff>
--- a/DatabaseStructure.xlsx
+++ b/DatabaseStructure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="145" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="291" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Column Name</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>char</t>
-  </si>
-  <si>
-    <t>Visitor</t>
   </si>
   <si>
     <t>Birthday</t>
@@ -186,15 +183,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -216,6 +213,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -353,7 +351,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -389,7 +387,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="R38" activeCellId="0" pane="topLeft" sqref="R38"/>
+      <selection activeCell="K16" activeCellId="0" pane="topLeft" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -459,33 +457,27 @@
         <v>13</v>
       </c>
       <c r="F5" s="7"/>
-      <c r="H5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="F6" s="7"/>
       <c r="H6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>10</v>
@@ -495,32 +487,32 @@
       </c>
       <c r="F7" s="7"/>
       <c r="H7" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="F8" s="7"/>
       <c r="H8" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="9">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>
@@ -530,16 +522,16 @@
       </c>
       <c r="F9" s="7"/>
       <c r="H9" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>10</v>
@@ -552,12 +544,13 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="E11" s="9" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F11" s="7"/>
@@ -567,7 +560,7 @@
       <c r="B12" s="6"/>
       <c r="F12" s="7"/>
       <c r="H12" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="13">
@@ -578,12 +571,12 @@
         <v>1</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
@@ -598,70 +591,71 @@
         <v>2</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="16">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="17">
       <c r="A17" s="2"/>
       <c r="B17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F17" s="7"/>
       <c r="H17" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="18">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="9" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F18" s="7"/>
@@ -669,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
@@ -684,34 +678,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="21">
       <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="22">
       <c r="A22" s="2"/>
       <c r="B22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>1</v>
@@ -722,7 +716,7 @@
       <c r="B23" s="6"/>
       <c r="F23" s="7"/>
       <c r="H23" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>2</v>
@@ -733,7 +727,7 @@
       <c r="B24" s="6"/>
       <c r="F24" s="7"/>
       <c r="H24" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>3</v>
@@ -741,10 +735,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="25">
       <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>10</v>
@@ -754,7 +748,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="H25" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>4</v>
@@ -765,7 +759,7 @@
       <c r="B26" s="6"/>
       <c r="F26" s="7"/>
       <c r="H26" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>5</v>
@@ -776,7 +770,7 @@
       <c r="B27" s="6"/>
       <c r="F27" s="7"/>
       <c r="H27" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>6</v>
@@ -784,7 +778,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="28">
       <c r="A28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>6</v>
@@ -796,7 +790,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>2</v>
@@ -805,7 +799,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="2"/>
       <c r="B29" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>10</v>
@@ -815,7 +809,7 @@
       </c>
       <c r="F29" s="7"/>
       <c r="H29" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>3</v>
@@ -826,7 +820,7 @@
       <c r="B30" s="6"/>
       <c r="F30" s="7"/>
       <c r="H30" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>4</v>
@@ -837,7 +831,7 @@
       <c r="B31" s="6"/>
       <c r="F31" s="7"/>
       <c r="H31" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>5</v>
@@ -845,7 +839,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="32">
       <c r="A32" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>6</v>
@@ -882,28 +876,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="2"/>
       <c r="B37" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
@@ -918,22 +912,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C40" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="7"/>
       <c r="B41" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>7</v>
@@ -941,7 +935,7 @@
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>